<commit_message>
ci: update confirmation formation form
</commit_message>
<xml_diff>
--- a/LF/Confirmation/Cote d'Ivoire/ci_202302_lf_conf_2_partcipants.xlsx
+++ b/LF/Confirmation/Cote d'Ivoire/ci_202302_lf_conf_2_partcipants.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\LF\TAS\Cote d'Ivoire\Fev 2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\LF\Confirmation\Cote d'Ivoire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBC2449-DFEA-4364-BA43-BE6369B770E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3F47D5-342A-4B6D-AF01-EA42DD8B4A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>p_eu_name</t>
-  </si>
-  <si>
     <t>Select your evaluation unit (EU)</t>
   </si>
   <si>
@@ -360,10 +357,13 @@
     <t>French</t>
   </si>
   <si>
-    <t>ci_202302_lf_tas1_2_partcipants</t>
-  </si>
-  <si>
-    <t>(2023 Dev) 2. TAS1 FL - Participants</t>
+    <t>(2023 Fev) 2. Recartographie FL - Participants</t>
+  </si>
+  <si>
+    <t>ci_202302_lf_conf_2_partcipants</t>
+  </si>
+  <si>
+    <t>p_region_name</t>
   </si>
 </sst>
 </file>
@@ -945,14 +945,14 @@
         <v>26</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="22"/>
       <c r="G3" s="12"/>
@@ -973,14 +973,14 @@
         <v>26</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="12"/>
@@ -1001,14 +1001,14 @@
         <v>26</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>34</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="12"/>
@@ -1029,14 +1029,14 @@
         <v>26</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="12"/>
@@ -1057,20 +1057,20 @@
         <v>26</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>39</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
       <c r="K7" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15" t="s">
@@ -1084,17 +1084,17 @@
         <v>26</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" s="9" t="s">
         <v>25</v>
@@ -1105,17 +1105,17 @@
         <v>26</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>25</v>
@@ -1123,17 +1123,17 @@
     </row>
     <row r="10" spans="1:16" s="3" customFormat="1">
       <c r="A10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="22"/>
       <c r="G10" s="13"/>
@@ -1151,17 +1151,17 @@
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1">
       <c r="A11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="13"/>
@@ -1169,7 +1169,7 @@
       <c r="I11" s="13"/>
       <c r="J11" s="12"/>
       <c r="K11" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13" t="s">
@@ -1184,28 +1184,28 @@
         <v>16</v>
       </c>
       <c r="B12" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>56</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="J12" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="13" t="s">
-        <v>60</v>
-      </c>
       <c r="K12" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" s="13"/>
       <c r="M12" s="13" t="s">
@@ -1220,28 +1220,28 @@
         <v>16</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="J13" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="J13" s="13" t="s">
-        <v>66</v>
-      </c>
       <c r="K13" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="13" t="s">
@@ -1256,32 +1256,32 @@
         <v>16</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="D14" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="E14" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="F14" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="J14" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="J14" s="15" t="s">
-        <v>74</v>
-      </c>
       <c r="K14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15" t="s">
@@ -1296,14 +1296,14 @@
         <v>26</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="12"/>
@@ -1311,10 +1311,10 @@
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>25</v>
@@ -1327,17 +1327,17 @@
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="31.5">
       <c r="A16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="12"/>
@@ -1345,7 +1345,7 @@
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L16" s="12"/>
       <c r="M16" s="13"/>
@@ -1355,17 +1355,17 @@
     </row>
     <row r="17" spans="1:16" s="3" customFormat="1">
       <c r="A17" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>85</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>86</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="12"/>
@@ -1381,10 +1381,10 @@
     </row>
     <row r="18" spans="1:16" s="3" customFormat="1">
       <c r="A18" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>88</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>89</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -1403,10 +1403,10 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -1448,7 +1448,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1463,86 +1463,86 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="D2" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>97</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1569,24 +1569,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>